<commit_message>
1. reran the HW1 code on single sharded index to reduce the scores
</commit_message>
<xml_diff>
--- a/HW_1/Summary.xlsx
+++ b/HW_1/Summary.xlsx
@@ -70,6 +70,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -92,12 +93,14 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -241,7 +244,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -299,7 +302,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0.3342</v>
+        <v>0.3</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0.416</v>
@@ -313,13 +316,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.3266</v>
+        <v>0.2962</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.408</v>
+        <v>0.42</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.34</v>
+        <v>0.3333</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -327,13 +330,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0.2758</v>
+        <v>0.225</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>0.364</v>
+        <v>0.42</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.3093</v>
+        <v>0.332</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added code for jelinek mercer smoothing with custom indexing
</commit_message>
<xml_diff>
--- a/HW_1/Summary.xlsx
+++ b/HW_1/Summary.xlsx
@@ -244,7 +244,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -344,13 +344,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0.242</v>
+        <v>0.236</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>0.356</v>
+        <v>0.368</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0.268</v>
+        <v>0.3093</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>